<commit_message>
Minor changes- Removed GB Bin Order
</commit_message>
<xml_diff>
--- a/Codes/All_Bins_Data.xlsx
+++ b/Codes/All_Bins_Data.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,15 +461,10 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>GB Bin Order</t>
+          <t>Bin Location</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Bin Location</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Availiability Flag</t>
         </is>
@@ -487,23 +482,20 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>140</v>
+        <v>269</v>
       </c>
       <c r="D2" t="n">
-        <v>2.36</v>
+        <v>4.548</v>
       </c>
       <c r="E2" t="n">
         <v>1</v>
       </c>
-      <c r="F2" t="n">
-        <v>0</v>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
       </c>
       <c r="G2" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
@@ -521,23 +513,20 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>273</v>
+        <v>393</v>
       </c>
       <c r="D3" t="n">
-        <v>195.7859999999997</v>
+        <v>297.9229999999996</v>
       </c>
       <c r="E3" t="n">
         <v>2</v>
       </c>
-      <c r="F3" t="n">
-        <v>0</v>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
       </c>
       <c r="G3" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
@@ -555,23 +544,20 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>330</v>
+        <v>302</v>
       </c>
       <c r="D4" t="n">
-        <v>329.9999999999999</v>
+        <v>302</v>
       </c>
       <c r="E4" t="n">
         <v>3</v>
       </c>
-      <c r="F4" t="n">
-        <v>0</v>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
       </c>
       <c r="G4" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
         <is>
           <t>No</t>
         </is>
@@ -589,25 +575,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>374</v>
+        <v>70</v>
       </c>
       <c r="D5" t="n">
-        <v>326.9400000000019</v>
+        <v>70.00000000000001</v>
       </c>
       <c r="E5" t="n">
         <v>4</v>
       </c>
-      <c r="F5" t="n">
-        <v>0</v>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -623,23 +606,20 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>236</v>
+        <v>211</v>
       </c>
       <c r="D6" t="n">
-        <v>235.991</v>
+        <v>211</v>
       </c>
       <c r="E6" t="n">
         <v>5</v>
       </c>
-      <c r="F6" t="n">
-        <v>0</v>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
       </c>
       <c r="G6" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
         <is>
           <t>No</t>
         </is>
@@ -657,25 +637,22 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>360</v>
+        <v>112</v>
       </c>
       <c r="D7" t="n">
-        <v>102.698</v>
+        <v>112</v>
       </c>
       <c r="E7" t="n">
         <v>6</v>
       </c>
-      <c r="F7" t="n">
-        <v>0</v>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -691,25 +668,22 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>299</v>
+        <v>186</v>
       </c>
       <c r="D8" t="n">
-        <v>1.75</v>
+        <v>185.9999999999999</v>
       </c>
       <c r="E8" t="n">
         <v>7</v>
       </c>
-      <c r="F8" t="n">
-        <v>0</v>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -725,23 +699,20 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>69</v>
+        <v>176</v>
       </c>
       <c r="D9" t="n">
-        <v>5.06</v>
+        <v>130.2160000000002</v>
       </c>
       <c r="E9" t="n">
         <v>8</v>
       </c>
-      <c r="F9" t="n">
-        <v>0</v>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
       </c>
       <c r="G9" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
@@ -759,23 +730,20 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>345</v>
+        <v>181</v>
       </c>
       <c r="D10" t="n">
-        <v>166.4300000000063</v>
+        <v>134.3900000000055</v>
       </c>
       <c r="E10" t="n">
         <v>9</v>
       </c>
-      <c r="F10" t="n">
-        <v>1</v>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
       </c>
       <c r="G10" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
@@ -793,23 +761,20 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>399</v>
+        <v>206</v>
       </c>
       <c r="D11" t="n">
-        <v>88.13800000000033</v>
+        <v>86.49100000000027</v>
       </c>
       <c r="E11" t="n">
         <v>10</v>
       </c>
-      <c r="F11" t="n">
-        <v>2</v>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
       </c>
       <c r="G11" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
@@ -827,25 +792,22 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>313</v>
+        <v>55</v>
       </c>
       <c r="D12" t="n">
-        <v>65.91500000000022</v>
+        <v>54.99500000000015</v>
       </c>
       <c r="E12" t="n">
         <v>11</v>
       </c>
-      <c r="F12" t="n">
-        <v>3</v>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -861,25 +823,22 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>50</v>
+        <v>212</v>
       </c>
       <c r="D13" t="n">
-        <v>49.99100000000001</v>
+        <v>52.99599999999997</v>
       </c>
       <c r="E13" t="n">
         <v>12</v>
       </c>
-      <c r="F13" t="n">
-        <v>4</v>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -895,25 +854,22 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>156</v>
+        <v>53</v>
       </c>
       <c r="D14" t="n">
-        <v>94.30000000000001</v>
+        <v>52.99900000000009</v>
       </c>
       <c r="E14" t="n">
         <v>13</v>
       </c>
-      <c r="F14" t="n">
-        <v>5</v>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -929,23 +885,20 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>318</v>
+        <v>208</v>
       </c>
       <c r="D15" t="n">
-        <v>46.483</v>
+        <v>57.87600000000001</v>
       </c>
       <c r="E15" t="n">
         <v>14</v>
       </c>
-      <c r="F15" t="n">
-        <v>6</v>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
       </c>
       <c r="G15" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
@@ -963,23 +916,20 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>196</v>
+        <v>382</v>
       </c>
       <c r="D16" t="n">
-        <v>0.806</v>
+        <v>7.804000000000002</v>
       </c>
       <c r="E16" t="n">
         <v>15</v>
       </c>
-      <c r="F16" t="n">
-        <v>7</v>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
       </c>
       <c r="G16" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
@@ -997,23 +947,20 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>383</v>
+        <v>127</v>
       </c>
       <c r="D17" t="n">
-        <v>0.474</v>
+        <v>2.945</v>
       </c>
       <c r="E17" t="n">
         <v>16</v>
       </c>
-      <c r="F17" t="n">
-        <v>8</v>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
       </c>
       <c r="G17" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
@@ -1031,23 +978,20 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>160</v>
+        <v>113</v>
       </c>
       <c r="D18" t="n">
-        <v>0.633</v>
+        <v>3.921</v>
       </c>
       <c r="E18" t="n">
         <v>17</v>
       </c>
-      <c r="F18" t="n">
-        <v>9</v>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
       </c>
       <c r="G18" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
@@ -1065,23 +1009,20 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>102</v>
+        <v>64</v>
       </c>
       <c r="D19" t="n">
-        <v>0</v>
+        <v>2.07</v>
       </c>
       <c r="E19" t="n">
         <v>18</v>
       </c>
-      <c r="F19" t="n">
-        <v>10</v>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
       </c>
       <c r="G19" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
@@ -1099,23 +1040,20 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>299</v>
+        <v>181</v>
       </c>
       <c r="D20" t="n">
-        <v>21.956</v>
+        <v>21.767</v>
       </c>
       <c r="E20" t="n">
         <v>19</v>
       </c>
-      <c r="F20" t="n">
-        <v>11</v>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
       </c>
       <c r="G20" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
@@ -1133,23 +1071,20 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>374</v>
+        <v>186</v>
       </c>
       <c r="D21" t="n">
-        <v>6.174</v>
+        <v>5.990999999999999</v>
       </c>
       <c r="E21" t="n">
         <v>20</v>
       </c>
-      <c r="F21" t="n">
-        <v>12</v>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
       </c>
       <c r="G21" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
@@ -1167,23 +1102,20 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>101</v>
+        <v>178</v>
       </c>
       <c r="D22" t="n">
-        <v>1.221</v>
+        <v>8.300999999999998</v>
       </c>
       <c r="E22" t="n">
         <v>21</v>
       </c>
-      <c r="F22" t="n">
-        <v>13</v>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
       </c>
       <c r="G22" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
@@ -1201,23 +1133,20 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>146</v>
+        <v>323</v>
       </c>
       <c r="D23" t="n">
-        <v>0.432</v>
+        <v>1.766</v>
       </c>
       <c r="E23" t="n">
         <v>22</v>
       </c>
-      <c r="F23" t="n">
-        <v>14</v>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
       </c>
       <c r="G23" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
@@ -1235,23 +1164,20 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>318</v>
+        <v>378</v>
       </c>
       <c r="D24" t="n">
-        <v>0.221</v>
+        <v>0.753</v>
       </c>
       <c r="E24" t="n">
         <v>23</v>
       </c>
-      <c r="F24" t="n">
-        <v>15</v>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
       </c>
       <c r="G24" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
@@ -1269,23 +1195,20 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>197</v>
+        <v>161</v>
       </c>
       <c r="D25" t="n">
-        <v>0</v>
+        <v>0.744</v>
       </c>
       <c r="E25" t="n">
         <v>24</v>
       </c>
-      <c r="F25" t="n">
-        <v>16</v>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
       </c>
       <c r="G25" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="H25" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
@@ -1303,23 +1226,20 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>161</v>
+        <v>214</v>
       </c>
       <c r="D26" t="n">
-        <v>0</v>
+        <v>0.183</v>
       </c>
       <c r="E26" t="n">
         <v>25</v>
       </c>
-      <c r="F26" t="n">
-        <v>17</v>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
       </c>
       <c r="G26" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="H26" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
@@ -1337,7 +1257,7 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>223</v>
+        <v>121</v>
       </c>
       <c r="D27" t="n">
         <v>0.248</v>
@@ -1345,15 +1265,12 @@
       <c r="E27" t="n">
         <v>26</v>
       </c>
-      <c r="F27" t="n">
-        <v>18</v>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
       </c>
       <c r="G27" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="H27" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
@@ -1371,23 +1288,20 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>78</v>
+        <v>233</v>
       </c>
       <c r="D28" t="n">
-        <v>6.613899999999997</v>
+        <v>6.613899999999998</v>
       </c>
       <c r="E28" t="n">
         <v>0</v>
       </c>
-      <c r="F28" t="n">
-        <v>0</v>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
       </c>
       <c r="G28" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="H28" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
@@ -1396,7 +1310,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>TR72</t>
+          <t>TR48</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1405,57 +1319,51 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="D29" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="E29" t="n">
         <v>0</v>
       </c>
-      <c r="F29" t="n">
-        <v>0</v>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>BC967248</t>
+          <t>TR72</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Bumper Cover</t>
+          <t>Tire</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>313</v>
+        <v>108</v>
       </c>
       <c r="D30" t="n">
-        <v>27.73579999999997</v>
+        <v>0</v>
       </c>
       <c r="E30" t="n">
         <v>0</v>
       </c>
-      <c r="F30" t="n">
-        <v>0</v>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
       </c>
       <c r="G30" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="H30" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
@@ -1464,32 +1372,29 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>BH967280</t>
+          <t>BC967248</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Hood</t>
+          <t>Bumper Cover</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D31" t="n">
-        <v>2.858500000000001</v>
+        <v>27.73579999999998</v>
       </c>
       <c r="E31" t="n">
         <v>0</v>
       </c>
-      <c r="F31" t="n">
-        <v>0</v>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
       </c>
       <c r="G31" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="H31" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
@@ -1498,41 +1403,38 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>HS06</t>
+          <t>BH967280</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Hanging</t>
+          <t>Hood</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>252</v>
+        <v>295</v>
       </c>
       <c r="D32" t="n">
-        <v>252</v>
+        <v>2.8585</v>
       </c>
       <c r="E32" t="n">
         <v>0</v>
       </c>
-      <c r="F32" t="n">
-        <v>0</v>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="H32" t="inlineStr">
-        <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>HS12</t>
+          <t>HS06</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1541,23 +1443,51 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>342</v>
+        <v>377</v>
       </c>
       <c r="D33" t="n">
-        <v>342</v>
+        <v>377</v>
       </c>
       <c r="E33" t="n">
         <v>0</v>
       </c>
-      <c r="F33" t="n">
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>HS12</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Hanging</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>364</v>
+      </c>
+      <c r="D34" t="n">
+        <v>364</v>
+      </c>
+      <c r="E34" t="n">
         <v>0</v>
       </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="H33" t="inlineStr">
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
         <is>
           <t>No</t>
         </is>

</xml_diff>